<commit_message>
Added Column Selection/Deselection feature
</commit_message>
<xml_diff>
--- a/documents/Published/DataInsights/DataInsightsByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/DataInsights/DataInsightsByMAQSoftwareChecklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PowerBICustomVisuals\documents\Published\DataInsights\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cutom Visual\PowerBI\documents\Published\DataInsights\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257AE7EF-0C33-4500-A079-B72777F743DD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3E2E9F2-9A7D-438E-95D9-E7E644CF52FB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1" xr2:uid="{0A959DB4-3E27-42B6-BC52-6DE114CB58CF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{0A959DB4-3E27-42B6-BC52-6DE114CB58CF}"/>
   </bookViews>
   <sheets>
     <sheet name="BVT" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="113">
   <si>
     <t>S no</t>
   </si>
@@ -44,16 +44,6 @@
   </si>
   <si>
     <t xml:space="preserve"> -</t>
-  </si>
-  <si>
-    <t>Top Menu bar is present with options
-1. View As
-2. Binning By
-3. X
-4. Y
-5. Color
-6. Text-Color
-7. Isolate</t>
   </si>
   <si>
     <t>Render visual for first time</t>
@@ -388,45 +378,59 @@
 4. Value dropdown</t>
   </si>
   <si>
-    <t>1. Fisrt 2 letters and ellipsis for the value in label is present on the brick in top left corner
+    <t>Coloumn selector button is present in the bottom of the visual.
+Top menu display only View as, Binning By, Color, Text color and Color By Button</t>
+  </si>
+  <si>
+    <t>Isolation is removed</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>visual not interactive</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Analytics Option is wrong</t>
+  </si>
+  <si>
+    <t>Show X Axis is wrong</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>Power BI</t>
+  </si>
+  <si>
+    <t>NO(In columnchart)</t>
+  </si>
+  <si>
+    <t>Top Menu bar is present with options
+1. View As
+2. Binning By
+3. X
+4. Y
+5. Color
+6. Text-Color</t>
+  </si>
+  <si>
+    <t>1. Now Brick header is same as the brick width
 2. Value is present in the bottom right corner
 3. If Binning By is not none then brick for each bin value are present</t>
   </si>
   <si>
-    <t>"1. Bar Chart is rendered for every Bin value
+    <t>1. Column Chart is rendered for every Bin value
+2. Width of bar chat is wrt  bin
+3. Added Selection/Deselection feature</t>
+  </si>
+  <si>
+    <t>1. Bar Chart is rendered for every Bin value
 2. Width of bar chat is wrt to Corresponding bin
-"</t>
-  </si>
-  <si>
-    <t>Coloumn selector button is present in the bottom of the visual.
-Top menu display only View as, Binning By, Color, Text color and Color By Button</t>
-  </si>
-  <si>
-    <t>Isolation is removed</t>
-  </si>
-  <si>
-    <t>YES</t>
-  </si>
-  <si>
-    <t>visual not interactive</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Analytics Option is wrong</t>
-  </si>
-  <si>
-    <t>Show X Axis is wrong</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>Power BI</t>
-  </si>
-  <si>
-    <t>NO(In columnchart)</t>
+3. Bar selection/deselection feature added</t>
   </si>
 </sst>
 </file>
@@ -477,10 +481,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -797,8 +801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD35E9AA-EC94-40B6-87B9-91903B6E03DF}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -827,16 +831,16 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="120" x14ac:dyDescent="0.25">
@@ -847,104 +851,104 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="G3" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="H3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="D5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="H3" t="s">
-        <v>97</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>99</v>
-      </c>
       <c r="G5" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="105" x14ac:dyDescent="0.25">
@@ -952,28 +956,28 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="D6" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="120" x14ac:dyDescent="0.25">
@@ -981,28 +985,28 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="D7" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="105" x14ac:dyDescent="0.25">
@@ -1010,28 +1014,28 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="D8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="F8" s="3" t="s">
-        <v>30</v>
+        <v>111</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1039,28 +1043,28 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="F9" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -1068,25 +1072,25 @@
         <v>7</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="F10" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="165" x14ac:dyDescent="0.25">
@@ -1094,62 +1098,62 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="D11" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="F12" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="D13" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1157,28 +1161,28 @@
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="F14" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1186,25 +1190,25 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>51</v>
-      </c>
       <c r="G15" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1212,48 +1216,48 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="E16" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="F16" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D17" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="F17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1261,28 +1265,28 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>91</v>
-      </c>
       <c r="F18" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1299,8 +1303,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA835CA9-E288-452C-87F2-A429070D6D1E}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1314,22 +1318,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" t="s">
         <v>58</v>
       </c>
-      <c r="B1" t="s">
-        <v>59</v>
-      </c>
       <c r="C1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>93</v>
+        <v>107</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1337,19 +1341,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1357,19 +1361,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>109</v>
+        <v>60</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1377,19 +1381,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>111</v>
+        <v>101</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1397,37 +1401,37 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F5" s="5"/>
+        <v>60</v>
+      </c>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1435,69 +1439,69 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F7" s="5"/>
+        <v>60</v>
+      </c>
+      <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="5"/>
+      <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F9" s="5"/>
+        <v>60</v>
+      </c>
+      <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C10" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1505,19 +1509,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C11" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1525,48 +1529,48 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F12" s="5"/>
+        <v>60</v>
+      </c>
+      <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="5"/>
+      <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C14" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1574,19 +1578,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C15" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>109</v>
+        <v>101</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1594,19 +1598,19 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>104</v>
+        <v>60</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1614,42 +1618,42 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="5" t="s">
-        <v>104</v>
+      <c r="F17" s="4" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E18" s="1"/>
-      <c r="F18" s="5" t="s">
-        <v>104</v>
+      <c r="F18" s="4" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C19" t="s">
+        <v>103</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="5" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1657,99 +1661,99 @@
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F20" s="5"/>
+        <v>60</v>
+      </c>
+      <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C21" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="5"/>
+      <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C23" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F23" s="5"/>
+        <v>104</v>
+      </c>
+      <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="5"/>
+      <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>19</v>
       </c>
       <c r="B26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C26" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1757,19 +1761,19 @@
         <v>20</v>
       </c>
       <c r="B27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C27" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>104</v>
+        <v>106</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>